<commit_message>
dados para calibracao volante
</commit_message>
<xml_diff>
--- a/sharedlib/OpenJAUS/medicoes na boca rodas.xlsx
+++ b/sharedlib/OpenJAUS/medicoes na boca rodas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="140" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
   <si>
     <t>Rodando o volante para o lado esquerdo (anti-horário)</t>
   </si>
@@ -282,6 +282,93 @@
   </si>
   <si>
     <t>35</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>trava</t>
+  </si>
+  <si>
+    <t>3929</t>
+  </si>
+  <si>
+    <t>4e4f</t>
+  </si>
+  <si>
+    <t>5822</t>
+  </si>
+  <si>
+    <t>4e4a</t>
+  </si>
+  <si>
+    <t>3935</t>
+  </si>
+  <si>
+    <t>4e5e</t>
+  </si>
+  <si>
+    <t>4e57</t>
+  </si>
+  <si>
+    <t>3a82</t>
+  </si>
+  <si>
+    <t>4fab</t>
+  </si>
+  <si>
+    <t>5976</t>
+  </si>
+  <si>
+    <t>4fa3</t>
+  </si>
+  <si>
+    <t>3924</t>
+  </si>
+  <si>
+    <t>4e61</t>
+  </si>
+  <si>
+    <t>4e54</t>
+  </si>
+  <si>
+    <t>37c8</t>
+  </si>
+  <si>
+    <t>4d0b</t>
+  </si>
+  <si>
+    <t>56c7</t>
+  </si>
+  <si>
+    <t>4d03</t>
+  </si>
+  <si>
+    <t>37ee</t>
+  </si>
+  <si>
+    <t>4d26</t>
+  </si>
+  <si>
+    <t>56e5</t>
+  </si>
+  <si>
+    <t>4d21</t>
+  </si>
+  <si>
+    <t>3979</t>
+  </si>
+  <si>
+    <t>4ea4</t>
+  </si>
+  <si>
+    <t>5868</t>
+  </si>
+  <si>
+    <t>4e95</t>
   </si>
 </sst>
 </file>
@@ -451,7 +538,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -486,7 +573,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -699,7 +786,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -896,7 +983,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1067,11 +1154,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="8158549"/>
-        <c:axId val="44055573"/>
+        <c:axId val="57990120"/>
+        <c:axId val="12854950"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="8158549"/>
+        <c:axId val="57990120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,11 +1175,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44055573"/>
+        <c:crossAx val="12854950"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44055573"/>
+        <c:axId val="12854950"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1119,7 +1206,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="8158549"/>
+        <c:crossAx val="57990120"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1159,15 +1246,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>297000</xdr:colOff>
+      <xdr:colOff>324000</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>86760</xdr:colOff>
+      <xdr:colOff>113400</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1175,8 +1262,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9265680" y="1950840"/>
-        <a:ext cx="10389240" cy="6357600"/>
+        <a:off x="9292680" y="1941840"/>
+        <a:ext cx="10388880" cy="6357240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1192,12 +1279,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1221,6 +1309,7 @@
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
+      <c r="L1" s="0"/>
       <c r="M1" s="0"/>
       <c r="N1" s="0"/>
       <c r="V1" s="0"/>
@@ -1238,6 +1327,7 @@
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
+      <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
       <c r="P2" s="3" t="s">
@@ -1417,6 +1507,7 @@
         <f aca="false">0.000000106681*E5*E5+0.00532682*E5-0.08083</f>
         <v>0.5064110401</v>
       </c>
+      <c r="L5" s="0"/>
       <c r="M5" s="0"/>
       <c r="N5" s="0"/>
       <c r="P5" s="2" t="s">
@@ -1488,6 +1579,7 @@
         <f aca="false">0.000000106681*E6*E6+0.00532682*E6-0.08083</f>
         <v>1.0962337604</v>
       </c>
+      <c r="L6" s="0"/>
       <c r="M6" s="0"/>
       <c r="N6" s="0"/>
       <c r="P6" s="2" t="s">
@@ -1559,6 +1651,7 @@
         <f aca="false">0.000000106681*E7*E7+0.00532682*E7-0.08083</f>
         <v>1.931729515625</v>
       </c>
+      <c r="L7" s="0"/>
       <c r="M7" s="0"/>
       <c r="N7" s="0"/>
       <c r="P7" s="2" t="s">
@@ -1630,6 +1723,7 @@
         <f aca="false">0.000000106681*E8*E8+0.00532682*E8-0.08083</f>
         <v>2.457195859904</v>
       </c>
+      <c r="L8" s="0"/>
       <c r="M8" s="0"/>
       <c r="N8" s="0"/>
       <c r="P8" s="2" t="s">
@@ -1701,6 +1795,7 @@
         <f aca="false">0.000000106681*E9*E9+0.00532682*E9-0.08083</f>
         <v>4.0291721456</v>
       </c>
+      <c r="L9" s="0"/>
       <c r="M9" s="0"/>
       <c r="N9" s="0"/>
       <c r="P9" s="2" t="s">
@@ -1772,6 +1867,7 @@
         <f aca="false">0.000000106681*E10*E10+0.00532682*E10-0.08083</f>
         <v>5.1865615529</v>
       </c>
+      <c r="L10" s="0"/>
       <c r="M10" s="0"/>
       <c r="N10" s="0"/>
       <c r="P10" s="2" t="s">
@@ -1843,6 +1939,7 @@
         <f aca="false">0.000000106681*E11*E11+0.00532682*E11-0.08083</f>
         <v>6.615789479249</v>
       </c>
+      <c r="L11" s="0"/>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
       <c r="P11" s="2" t="s">
@@ -1914,6 +2011,7 @@
         <f aca="false">0.000000106681*E12*E12+0.00532682*E12-0.08083</f>
         <v>8.0365376624</v>
       </c>
+      <c r="L12" s="0"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
       <c r="P12" s="2" t="s">
@@ -1985,6 +2083,7 @@
         <f aca="false">0.000000106681*E13*E13+0.00532682*E13-0.08083</f>
         <v>9.294451587524</v>
       </c>
+      <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
       <c r="P13" s="2" t="s">
@@ -2056,6 +2155,7 @@
         <f aca="false">0.000000106681*E14*E14+0.00532682*E14-0.08083</f>
         <v>10.236199728209</v>
       </c>
+      <c r="L14" s="0"/>
       <c r="M14" s="0"/>
       <c r="N14" s="0"/>
       <c r="P14" s="2" t="s">
@@ -2127,6 +2227,7 @@
         <f aca="false">0.000000106681*E15*E15+0.00532682*E15-0.08083</f>
         <v>12.15451004</v>
       </c>
+      <c r="L15" s="0"/>
       <c r="M15" s="0"/>
       <c r="N15" s="0"/>
       <c r="P15" s="2" t="s">
@@ -2198,6 +2299,7 @@
         <f aca="false">0.000000106681*E16*E16+0.00532682*E16-0.08083</f>
         <v>13.31802056</v>
       </c>
+      <c r="L16" s="0"/>
       <c r="M16" s="0"/>
       <c r="N16" s="0"/>
       <c r="P16" s="2" t="s">
@@ -2269,6 +2371,7 @@
         <f aca="false">0.000000106681*E17*E17+0.00532682*E17-0.08083</f>
         <v>14.578312981225</v>
       </c>
+      <c r="L17" s="0"/>
       <c r="M17" s="0"/>
       <c r="N17" s="0"/>
       <c r="P17" s="2" t="s">
@@ -2340,6 +2443,7 @@
         <f aca="false">0.000000106681*E18*E18+0.00532682*E18-0.08083</f>
         <v>15.878123900225</v>
       </c>
+      <c r="L18" s="0"/>
       <c r="M18" s="0"/>
       <c r="N18" s="0"/>
       <c r="P18" s="2" t="s">
@@ -2411,6 +2515,7 @@
         <f aca="false">0.000000106681*E19*E19+0.00532682*E19-0.08083</f>
         <v>17.140439240329</v>
       </c>
+      <c r="L19" s="0"/>
       <c r="M19" s="0"/>
       <c r="N19" s="0"/>
       <c r="P19" s="2" t="s">
@@ -2482,6 +2587,7 @@
         <f aca="false">0.000000106681*E20*E20+0.00532682*E20-0.08083</f>
         <v>18.810271630625</v>
       </c>
+      <c r="L20" s="0"/>
       <c r="M20" s="0"/>
       <c r="N20" s="0"/>
       <c r="P20" s="2" t="s">
@@ -2553,6 +2659,7 @@
         <f aca="false">0.000000106681*E21*E21+0.00532682*E21-0.08083</f>
         <v>20.1129964196</v>
       </c>
+      <c r="L21" s="0"/>
       <c r="M21" s="0"/>
       <c r="N21" s="0"/>
       <c r="P21" s="2" t="s">
@@ -2624,6 +2731,7 @@
         <f aca="false">0.000000106681*E22*E22+0.00532682*E22-0.08083</f>
         <v>21.192874130609</v>
       </c>
+      <c r="L22" s="0"/>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
       <c r="P22" s="2" t="s">
@@ -2695,6 +2803,7 @@
         <f aca="false">0.000000106681*E23*E23+0.00532682*E23-0.08083</f>
         <v>22.532079307225</v>
       </c>
+      <c r="L23" s="0"/>
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
       <c r="P23" s="2" t="s">
@@ -2766,6 +2875,7 @@
         <f aca="false">0.000000106681*E24*E24+0.00532682*E24-0.08083</f>
         <v>24.372910174144</v>
       </c>
+      <c r="L24" s="0"/>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
     </row>
@@ -2809,6 +2919,7 @@
         <f aca="false">0.000000106681*E25*E25+0.00532682*E25-0.08083</f>
         <v>25.8616377929</v>
       </c>
+      <c r="L25" s="0"/>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
     </row>
@@ -2852,6 +2963,7 @@
         <f aca="false">0.000000106681*E26*E26+0.00532682*E26-0.08083</f>
         <v>27.768093065104</v>
       </c>
+      <c r="L26" s="0"/>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
     </row>
@@ -2895,6 +3007,7 @@
         <f aca="false">0.000000106681*E27*E27+0.00532682*E27-0.08083</f>
         <v>29.905634800769</v>
       </c>
+      <c r="L27" s="0"/>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
     </row>
@@ -2944,6 +3057,139 @@
       </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
impletacao da calibracao do angulo do volante
</commit_message>
<xml_diff>
--- a/sharedlib/OpenJAUS/medicoes na boca rodas.xlsx
+++ b/sharedlib/OpenJAUS/medicoes na boca rodas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
   <si>
     <t>Rodando o volante para o lado esquerdo (anti-horário)</t>
   </si>
@@ -293,6 +293,12 @@
     <t>trava</t>
   </si>
   <si>
+    <t>zero1</t>
+  </si>
+  <si>
+    <t>zero2</t>
+  </si>
+  <si>
     <t>3929</t>
   </si>
   <si>
@@ -369,17 +375,42 @@
   </si>
   <si>
     <t>4e95</t>
+  </si>
+  <si>
+    <t>zero1-limit</t>
+  </si>
+  <si>
+    <t>trava-limit</t>
+  </si>
+  <si>
+    <t>zero2-limit</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>zero1-zero2</t>
+  </si>
+  <si>
+    <t>trava-zero1</t>
+  </si>
+  <si>
+    <t>trava-zero2</t>
+  </si>
+  <si>
+    <t>Para calibrar basta ir até o limite no sentido horário e depois voltar no sentido antiorário até a “trava”. O zero está 2500 no sentido anti-horario a partir da trava.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -400,6 +431,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -449,7 +487,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -464,6 +502,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -573,7 +619,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -786,7 +832,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -983,7 +1029,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1154,11 +1200,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="57990120"/>
-        <c:axId val="12854950"/>
+        <c:axId val="32599814"/>
+        <c:axId val="48845857"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57990120"/>
+        <c:axId val="32599814"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,11 +1221,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="12854950"/>
+        <c:crossAx val="48845857"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="12854950"/>
+        <c:axId val="48845857"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1252,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="57990120"/>
+        <c:crossAx val="32599814"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1246,15 +1292,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>324000</xdr:colOff>
+      <xdr:colOff>351360</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>113400</xdr:colOff>
+      <xdr:colOff>140400</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1262,8 +1308,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9292680" y="1941840"/>
-        <a:ext cx="10388880" cy="6357240"/>
+        <a:off x="9495720" y="1932840"/>
+        <a:ext cx="10388520" cy="6321600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1279,19 +1325,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="2" style="1" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="2" style="1" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.0459183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="11.5561224489796"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.5561224489796"/>
     <col collapsed="false" hidden="false" max="15" min="12" style="1" width="11.5561224489796"/>
     <col collapsed="false" hidden="false" max="21" min="16" style="0" width="11.5561224489796"/>
@@ -3058,6 +3106,24 @@
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
     </row>
+    <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+    </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
         <v>89</v>
@@ -3071,22 +3137,53 @@
       <c r="E32" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="G32" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <f aca="false">HEX2DEC(B33)</f>
+        <v>14633</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <f aca="false">HEX2DEC(C33)</f>
+        <v>20047</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <f aca="false">HEX2DEC(D33)</f>
+        <v>22562</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <f aca="false">HEX2DEC(E33)</f>
+        <v>20042</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3094,16 +3191,35 @@
         <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <f aca="false">HEX2DEC(B34)</f>
+        <v>14645</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <f aca="false">HEX2DEC(C34)</f>
+        <v>20062</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <f aca="false">HEX2DEC(D34)</f>
+        <v>22562</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <f aca="false">HEX2DEC(E34)</f>
+        <v>20055</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,16 +3227,35 @@
         <v>3</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <f aca="false">HEX2DEC(B35)</f>
+        <v>14978</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <f aca="false">HEX2DEC(C35)</f>
+        <v>20395</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <f aca="false">HEX2DEC(D35)</f>
+        <v>22902</v>
+      </c>
+      <c r="J35" s="1" t="n">
+        <f aca="false">HEX2DEC(E35)</f>
+        <v>20387</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3128,16 +3263,35 @@
         <v>4</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <f aca="false">HEX2DEC(B36)</f>
+        <v>14628</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <f aca="false">HEX2DEC(C36)</f>
+        <v>20065</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <f aca="false">HEX2DEC(D36)</f>
+        <v>22562</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <f aca="false">HEX2DEC(E36)</f>
+        <v>20052</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3145,16 +3299,35 @@
         <v>5</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <f aca="false">HEX2DEC(B37)</f>
+        <v>14280</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <f aca="false">HEX2DEC(C37)</f>
+        <v>19723</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <f aca="false">HEX2DEC(D37)</f>
+        <v>22215</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <f aca="false">HEX2DEC(E37)</f>
+        <v>19715</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3162,16 +3335,35 @@
         <v>6</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <f aca="false">HEX2DEC(B38)</f>
+        <v>14318</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <f aca="false">HEX2DEC(C38)</f>
+        <v>19750</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <f aca="false">HEX2DEC(D38)</f>
+        <v>22245</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <f aca="false">HEX2DEC(E38)</f>
+        <v>19745</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3179,16 +3371,297 @@
         <v>7</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <f aca="false">HEX2DEC(B39)</f>
+        <v>14713</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <f aca="false">HEX2DEC(C39)</f>
+        <v>20132</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <f aca="false">HEX2DEC(D39)</f>
+        <v>22632</v>
+      </c>
+      <c r="J39" s="1" t="n">
+        <f aca="false">HEX2DEC(E39)</f>
+        <v>20117</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H43" s="1" t="n">
+        <f aca="false">H33-G33</f>
+        <v>5414</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <f aca="false">I33-G33</f>
+        <v>7929</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <f aca="false">J33-G33</f>
+        <v>5409</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H44" s="1" t="n">
+        <f aca="false">H34-G34</f>
+        <v>5417</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <f aca="false">I34-G34</f>
+        <v>7917</v>
+      </c>
+      <c r="J44" s="1" t="n">
+        <f aca="false">J34-G34</f>
+        <v>5410</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H45" s="1" t="n">
+        <f aca="false">H35-G35</f>
+        <v>5417</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <f aca="false">I35-G35</f>
+        <v>7924</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <f aca="false">J35-G35</f>
+        <v>5409</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H46" s="1" t="n">
+        <f aca="false">H36-G36</f>
+        <v>5437</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <f aca="false">I36-G36</f>
+        <v>7934</v>
+      </c>
+      <c r="J46" s="1" t="n">
+        <f aca="false">J36-G36</f>
+        <v>5424</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H47" s="1" t="n">
+        <f aca="false">H37-G37</f>
+        <v>5443</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <f aca="false">I37-G37</f>
+        <v>7935</v>
+      </c>
+      <c r="J47" s="1" t="n">
+        <f aca="false">J37-G37</f>
+        <v>5435</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H48" s="1" t="n">
+        <f aca="false">H38-G38</f>
+        <v>5432</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <f aca="false">I38-G38</f>
+        <v>7927</v>
+      </c>
+      <c r="J48" s="1" t="n">
+        <f aca="false">J38-G38</f>
+        <v>5427</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H49" s="1" t="n">
+        <f aca="false">H39-G39</f>
+        <v>5419</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <f aca="false">I39-G39</f>
+        <v>7919</v>
+      </c>
+      <c r="J49" s="1" t="n">
+        <f aca="false">J39-G39</f>
+        <v>5404</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G50" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H50" s="5" t="n">
+        <f aca="false">AVERAGE(H43:H49)</f>
+        <v>5425.57142857143</v>
+      </c>
+      <c r="I50" s="5" t="n">
+        <f aca="false">AVERAGE(I43:I49)</f>
+        <v>7926.42857142857</v>
+      </c>
+      <c r="J50" s="5" t="n">
+        <f aca="false">AVERAGE(J43:J49)</f>
+        <v>5416.85714285714</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I51" s="0"/>
+      <c r="J51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H53" s="1" t="n">
+        <f aca="false">H33-J33</f>
+        <v>5</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <f aca="false">I33-H33</f>
+        <v>2515</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <f aca="false">I33-J33</f>
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H54" s="1" t="n">
+        <f aca="false">H34-J34</f>
+        <v>7</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <f aca="false">I34-H34</f>
+        <v>2500</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <f aca="false">I34-J34</f>
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H55" s="1" t="n">
+        <f aca="false">H35-J35</f>
+        <v>8</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <f aca="false">I35-H35</f>
+        <v>2507</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <f aca="false">I35-J35</f>
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H56" s="1" t="n">
+        <f aca="false">H36-J36</f>
+        <v>13</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <f aca="false">I36-H36</f>
+        <v>2497</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <f aca="false">I36-J36</f>
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H57" s="1" t="n">
+        <f aca="false">H37-J37</f>
+        <v>8</v>
+      </c>
+      <c r="I57" s="1" t="n">
+        <f aca="false">I37-H37</f>
+        <v>2492</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <f aca="false">I37-J37</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H58" s="1" t="n">
+        <f aca="false">H38-J38</f>
+        <v>5</v>
+      </c>
+      <c r="I58" s="1" t="n">
+        <f aca="false">I38-H38</f>
+        <v>2495</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <f aca="false">I38-J38</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H59" s="1" t="n">
+        <f aca="false">H39-J39</f>
+        <v>15</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <f aca="false">I39-H39</f>
+        <v>2500</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <f aca="false">I39-J39</f>
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G60" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H60" s="5" t="n">
+        <f aca="false">AVERAGE(H53:H59)</f>
+        <v>8.71428571428571</v>
+      </c>
+      <c r="I60" s="5" t="n">
+        <f aca="false">AVERAGE(I53:I59)</f>
+        <v>2500.85714285714</v>
+      </c>
+      <c r="J60" s="5" t="n">
+        <f aca="false">AVERAGE(J53:J59)</f>
+        <v>2509.57142857143</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
melhorias no zero do esforco do volante
</commit_message>
<xml_diff>
--- a/sharedlib/OpenJAUS/medicoes na boca rodas.xlsx
+++ b/sharedlib/OpenJAUS/medicoes na boca rodas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="140" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="76" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -619,7 +619,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -832,7 +832,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1029,7 +1029,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1200,11 +1200,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="32599814"/>
-        <c:axId val="48845857"/>
+        <c:axId val="68439133"/>
+        <c:axId val="69799739"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32599814"/>
+        <c:axId val="68439133"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,11 +1221,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48845857"/>
+        <c:crossAx val="69799739"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48845857"/>
+        <c:axId val="69799739"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1252,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="32599814"/>
+        <c:crossAx val="68439133"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1292,15 +1292,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>351360</xdr:colOff>
+      <xdr:colOff>378360</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>140400</xdr:colOff>
+      <xdr:colOff>167040</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1308,8 +1308,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9495720" y="1932840"/>
-        <a:ext cx="10388520" cy="6321600"/>
+        <a:off x="9522720" y="1923840"/>
+        <a:ext cx="10388160" cy="6321240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1328,9 +1328,9 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W62"/>
+  <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
@@ -3111,18 +3111,33 @@
       <c r="C29" s="0"/>
       <c r="D29" s="0"/>
       <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0"/>
       <c r="C30" s="0"/>
       <c r="D30" s="0"/>
       <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0"/>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
       <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
@@ -3137,6 +3152,7 @@
       <c r="E32" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="F32" s="0"/>
       <c r="G32" s="2" t="s">
         <v>89</v>
       </c>
@@ -3402,8 +3418,20 @@
         <v>20117</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
+      <c r="I40" s="0"/>
+      <c r="J40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
+      <c r="J41" s="0"/>
+    </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="0"/>
       <c r="H42" s="2" t="s">
         <v>120</v>
       </c>
@@ -3415,6 +3443,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="0"/>
       <c r="H43" s="1" t="n">
         <f aca="false">H33-G33</f>
         <v>5414</v>
@@ -3429,6 +3458,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G44" s="0"/>
       <c r="H44" s="1" t="n">
         <f aca="false">H34-G34</f>
         <v>5417</v>
@@ -3443,6 +3473,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G45" s="0"/>
       <c r="H45" s="1" t="n">
         <f aca="false">H35-G35</f>
         <v>5417</v>
@@ -3457,6 +3488,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G46" s="0"/>
       <c r="H46" s="1" t="n">
         <f aca="false">H36-G36</f>
         <v>5437</v>
@@ -3471,6 +3503,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G47" s="0"/>
       <c r="H47" s="1" t="n">
         <f aca="false">H37-G37</f>
         <v>5443</v>
@@ -3485,6 +3518,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G48" s="0"/>
       <c r="H48" s="1" t="n">
         <f aca="false">H38-G38</f>
         <v>5432</v>
@@ -3499,6 +3533,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G49" s="0"/>
       <c r="H49" s="1" t="n">
         <f aca="false">H39-G39</f>
         <v>5419</v>
@@ -3530,10 +3565,13 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="0"/>
+      <c r="H51" s="0"/>
       <c r="I51" s="0"/>
       <c r="J51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="0"/>
       <c r="H52" s="1" t="s">
         <v>124</v>
       </c>
@@ -3545,6 +3583,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G53" s="0"/>
       <c r="H53" s="1" t="n">
         <f aca="false">H33-J33</f>
         <v>5</v>
@@ -3559,6 +3598,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G54" s="0"/>
       <c r="H54" s="1" t="n">
         <f aca="false">H34-J34</f>
         <v>7</v>
@@ -3573,6 +3613,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G55" s="0"/>
       <c r="H55" s="1" t="n">
         <f aca="false">H35-J35</f>
         <v>8</v>
@@ -3587,6 +3628,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G56" s="0"/>
       <c r="H56" s="1" t="n">
         <f aca="false">H36-J36</f>
         <v>13</v>
@@ -3601,6 +3643,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G57" s="0"/>
       <c r="H57" s="1" t="n">
         <f aca="false">H37-J37</f>
         <v>8</v>
@@ -3615,6 +3658,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G58" s="0"/>
       <c r="H58" s="1" t="n">
         <f aca="false">H38-J38</f>
         <v>5</v>
@@ -3629,6 +3673,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G59" s="0"/>
       <c r="H59" s="1" t="n">
         <f aca="false">H39-J39</f>
         <v>15</v>
@@ -3662,6 +3707,11 @@
     <row r="62" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>